<commit_message>
feat: add user UI
</commit_message>
<xml_diff>
--- a/Out/OPCIONES PARA CSE - 1.xlsx
+++ b/Out/OPCIONES PARA CSE - 1.xlsx
@@ -525,25 +525,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -553,25 +553,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -581,25 +581,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -609,25 +609,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -647,17 +647,9 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
     </row>
@@ -667,17 +659,9 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -687,17 +671,9 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -708,17 +684,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -728,17 +696,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -748,17 +708,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -768,17 +720,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -787,17 +731,9 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
     </row>
@@ -807,17 +743,9 @@
           <t>15:30</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
     </row>
@@ -829,13 +757,13 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -849,13 +777,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -867,9 +795,17 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
@@ -915,9 +851,17 @@
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -927,9 +871,17 @@
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -939,9 +891,17 @@
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
@@ -951,9 +911,17 @@
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -1049,7 +1017,11 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1061,7 +1033,11 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1073,7 +1049,11 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1085,7 +1065,11 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1093,27 +1077,15 @@
           <t>09:00</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1121,27 +1093,15 @@
           <t>09:30</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1149,26 +1109,10 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -1177,26 +1121,10 @@
           <t>10:30</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1206,10 +1134,26 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1217,19 +1161,27 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1237,19 +1189,27 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1257,19 +1217,27 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1278,17 +1246,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1298,17 +1258,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -1318,17 +1270,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -1338,17 +1282,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1405,9 +1341,17 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
@@ -1417,9 +1361,17 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -1429,9 +1381,17 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
@@ -1441,9 +1401,17 @@
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -1453,17 +1421,9 @@
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -1473,17 +1433,9 @@
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -1493,17 +1445,9 @@
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
@@ -1513,17 +1457,9 @@
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS4]</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -1615,9 +1551,17 @@
           <t>07:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
     </row>
@@ -1627,9 +1571,17 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
     </row>
@@ -1639,9 +1591,17 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>
@@ -1651,9 +1611,17 @@
           <t>08:30</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -1665,25 +1633,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1693,25 +1661,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1721,25 +1689,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1749,25 +1717,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1787,17 +1755,9 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
     </row>
@@ -1807,17 +1767,9 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -1827,17 +1779,9 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED1]</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -1848,17 +1792,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1868,17 +1804,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -1888,17 +1816,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -1908,17 +1828,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1951,9 +1863,17 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
@@ -1963,9 +1883,17 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -1977,13 +1905,13 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1995,17 +1923,9 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -2015,17 +1935,9 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
@@ -2035,17 +1947,9 @@
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -2186,17 +2090,9 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2206,17 +2102,9 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -2226,17 +2114,9 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -2259,25 +2139,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2287,25 +2167,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2315,25 +2195,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2343,25 +2223,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2381,9 +2261,17 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
     </row>
@@ -2393,9 +2281,17 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -2405,9 +2301,17 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -2418,17 +2322,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -2438,17 +2334,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -2458,17 +2346,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -2478,17 +2358,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -2497,17 +2369,9 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
     </row>
@@ -2517,17 +2381,9 @@
           <t>15:30</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
     </row>
@@ -2537,17 +2393,9 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
@@ -2557,17 +2405,9 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -2625,9 +2465,17 @@
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -2637,9 +2485,17 @@
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -2649,9 +2505,17 @@
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
@@ -2661,9 +2525,17 @@
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -2755,18 +2627,18 @@
           <t>07:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2775,18 +2647,18 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -2795,18 +2667,18 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -2815,9 +2687,17 @@
           <t>08:30</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -2829,25 +2709,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2857,25 +2737,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2885,25 +2765,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2913,25 +2793,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2951,9 +2831,17 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
     </row>
@@ -2963,9 +2851,17 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -2975,9 +2871,17 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED4]</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -2988,17 +2892,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -3008,17 +2904,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -3028,17 +2916,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -3048,17 +2928,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3115,17 +2987,9 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
@@ -3135,17 +2999,9 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -3155,17 +3011,9 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
@@ -3175,17 +3023,9 @@
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -3375,25 +3215,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3403,25 +3243,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -3431,25 +3271,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -3459,25 +3299,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -3499,13 +3339,13 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -3519,13 +3359,13 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -3539,13 +3379,13 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>REDACCIÓN [RED1]</t>
+          <t>REDACCIÓN [RED4]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -3557,26 +3397,10 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -3585,26 +3409,10 @@
           <t>13:30</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -3613,26 +3421,10 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -3641,26 +3433,10 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3717,9 +3493,17 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
@@ -3729,9 +3513,17 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -3741,9 +3533,17 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
@@ -3753,9 +3553,17 @@
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS6]</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -3896,17 +3704,9 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -3916,17 +3716,9 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -3936,17 +3728,9 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -3967,26 +3751,10 @@
           <t>09:00</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -3995,26 +3763,10 @@
           <t>09:30</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -4023,26 +3775,10 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -4051,26 +3787,10 @@
           <t>10:30</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA1]</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -4080,10 +3800,26 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -4092,10 +3828,26 @@
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -4104,10 +3856,26 @@
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -4116,10 +3884,26 @@
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -4127,26 +3911,10 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -4155,26 +3923,10 @@
           <t>13:30</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -4183,26 +3935,10 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -4211,26 +3947,10 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -4263,9 +3983,17 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
@@ -4275,9 +4003,17 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -4287,9 +4023,17 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
@@ -4335,9 +4079,17 @@
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -4347,9 +4099,17 @@
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -4359,9 +4119,17 @@
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
@@ -4371,9 +4139,17 @@
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -4466,18 +4242,14 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -4486,18 +4258,14 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -4506,18 +4274,14 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -4529,7 +4293,11 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -4541,7 +4309,11 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -4553,7 +4325,11 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -4585,27 +4361,27 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -4613,27 +4389,27 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -4641,27 +4417,27 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -4669,27 +4445,27 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -4698,17 +4474,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -4718,17 +4486,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -4738,17 +4498,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -4758,17 +4510,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -4777,17 +4521,9 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
     </row>
@@ -4797,17 +4533,9 @@
           <t>15:30</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
     </row>
@@ -4817,17 +4545,9 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
@@ -4837,17 +4557,9 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS2]</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -4905,9 +4617,17 @@
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -4917,9 +4637,17 @@
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -4929,9 +4657,17 @@
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
@@ -4941,9 +4677,17 @@
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS8]</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -5035,18 +4779,18 @@
           <t>07:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -5055,18 +4799,18 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -5075,18 +4819,18 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -5095,9 +4839,17 @@
           <t>08:30</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -5155,27 +4907,27 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -5183,27 +4935,27 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -5211,27 +4963,27 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -5239,27 +4991,27 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -5268,17 +5020,9 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -5288,17 +5032,9 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -5308,17 +5044,9 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -5328,17 +5056,9 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -5371,9 +5091,17 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
@@ -5383,9 +5111,17 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED6]</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -5397,13 +5133,13 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
+          <t>REDACCIÓN [RED6]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -5415,17 +5151,9 @@
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -5435,17 +5163,9 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
@@ -5455,17 +5175,9 @@
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS3]</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -5605,19 +5317,23 @@
           <t>07:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -5625,19 +5341,23 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -5645,19 +5365,23 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>REDACCIÓN [RED2]</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>REDACCIÓN [RED2]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -5665,11 +5389,23 @@
           <t>08:30</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -5681,7 +5417,11 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -5693,7 +5433,11 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>REDACCIÓN [RED2]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -5725,27 +5469,27 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -5753,27 +5497,27 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -5781,27 +5525,27 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -5809,27 +5553,27 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ÁLGEBRA AMPLIADA [ALA2]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ÁLGEBRA AMPLIADA [ALA6]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -5837,26 +5581,10 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -5865,26 +5593,10 @@
           <t>13:30</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -5893,26 +5605,10 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -5921,26 +5617,10 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INTRODUCCIÓN A LA FÍSICA /FÍSICA /FUND CIENT PARA INGENIERÍA [FIS1]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ANÁLISIS Y DISEÑO DE ALGORITMOS [ADA3]</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">

</xml_diff>